<commit_message>
[P10-0001] - Refatoração das classes Despacho, FrenteColheita; - Criação de arquivos separados, contendo lógica de criação de tela; - Criação do arquivo constantes, contendo contantes que serão utilizadas no projeto;
</commit_message>
<xml_diff>
--- a/equipamentos.xlsx
+++ b/equipamentos.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -505,6 +505,25 @@
         </is>
       </c>
     </row>
+    <row r="7"/>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>